<commit_message>
Added more datasets and modified the model on the main notebook. Also created new files just to make tests.
</commit_message>
<xml_diff>
--- a/predicciones_cupos_proximo_semestre.xlsx
+++ b/predicciones_cupos_proximo_semestre.xlsx
@@ -448,267 +448,267 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADMINISTRACION DE BASES DE DATOS</t>
+          <t>MATEMATICA DISCRETA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>71</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ADMINISTRACION DE REDES</t>
+          <t>METODOS MATEMATICOS I</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ADMINISTRACION DE SERVIDORES</t>
+          <t>PROGRAMACION</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>43</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ALGORITMIA</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE PROGRAMACION</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>37</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ALMACENES DE DATOS (DATA WAREHOUSE)</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS I</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>48</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BASES DE DATOS</t>
+          <t>ALGORITMIA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CLASIFICACION INTELIGENTE DE DATOS</t>
+          <t>ESTRUCTURAS DE DATOS I</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>58</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CONTROL DE PROYECTOS</t>
+          <t>METODOS MATEMATICOS II</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>61</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ESTADISTICA Y PROCESOS ESTOCASTICOS</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ALGORITMIA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>81</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ESTRUCTURAS DE DATOS I</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS I</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ESTRUCTURAS DE DATOS II</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS II</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>14</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>HIPERMEDIA</t>
+          <t>ADMINISTRACION DE REDES</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>41</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>INGENIERIA DE SOFTWARE I</t>
+          <t>ESTADISTICA Y PROCESOS ESTOCASTICOS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>11</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>INGENIERIA DE SOFTWARE II</t>
+          <t>ESTRUCTURAS DE DATOS II</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MATEMATICA DISCRETA</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS II</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>METODOS MATEMATICOS I</t>
+          <t>TEORIA DE LA COMPUTACION</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>114</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>METODOS MATEMATICOS II</t>
+          <t>ADMINISTRACION DE SERVIDORES</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MINERIA DE DATOS</t>
+          <t>BASES DE DATOS</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PROGRAMACION</t>
+          <t>HIPERMEDIA</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>106</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PROGRAMACION PARA INTERNET</t>
+          <t>INGENIERIA DE SOFTWARE I</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>154</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SEGURIDAD DE LA INFORMACION</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE BASES DE DATOS</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>80</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE BASES DE DATOS</t>
+          <t>CONTROL DE PROYECTOS</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>71</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE PROGRAMACION</t>
+          <t>INGENIERIA DE SOFTWARE II</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ALGORITMIA</t>
+          <t>PROGRAMACION PARA INTERNET</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>76</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS I</t>
+          <t>SEGURIDAD DE LA INFORMACION</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>11</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS II</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE INGENIERIA DE SOFTWARE I</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>34</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS I</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE USO, ADAPTACION, EXPLOTACION DE SISTEMAS OPERATIVOS</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -718,71 +718,71 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS II</t>
+          <t>USO, ADAPTACION Y EXPLOTACION DE SISTEMAS OPERATIVOS</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>91</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE INGENIERIA DE SOFTWARE I</t>
+          <t>ADMINISTRACION DE BASES DE DATOS</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE USO, ADAPTACION, EXPLOTACION DE SISTEMAS OPERATIVOS</t>
+          <t>ALMACENES DE DATOS (DATA WAREHOUSE)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE SISTEMAS BASADOS EN CONOCIMIENTO</t>
+          <t>MINERIA DE DATOS</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>62</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SISTEMAS BASADOS EN CONOCIMIENTO</t>
+          <t>CLASIFICACION INTELIGENTE DE DATOS</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>63</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>TEORIA DE LA COMPUTACION</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE SISTEMAS BASADOS EN CONOCIMIENTO</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>32</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>USO, ADAPTACION Y EXPLOTACION DE SISTEMAS OPERATIVOS</t>
+          <t>SISTEMAS BASADOS EN CONOCIMIENTO</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>70</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing XGBOOST model and Random Forest
</commit_message>
<xml_diff>
--- a/predicciones_cupos_proximo_semestre.xlsx
+++ b/predicciones_cupos_proximo_semestre.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,344 +448,334 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MATEMATICA DISCRETA</t>
+          <t>ADMINISTRACION DE BASES DE DATOS</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>44</v>
+        <v>143.9074096679688</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>METODOS MATEMATICOS I</t>
+          <t>ADMINISTRACION DE REDES</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>130</v>
+        <v>121.9426116943359</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PROGRAMACION</t>
+          <t>ADMINISTRACION DE SERVIDORES</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>121</v>
+        <v>144.1614990234375</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE PROGRAMACION</t>
+          <t>ALGORITMIA</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>129</v>
+        <v>133.6002960205078</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS I</t>
+          <t>ALMACENES DE DATOS (DATA WAREHOUSE)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>166</v>
+        <v>151.3702545166016</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ALGORITMIA</t>
+          <t>BASES DE DATOS</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>57</v>
+        <v>152.0135345458984</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ESTRUCTURAS DE DATOS I</t>
+          <t>CLASIFICACION INTELIGENTE DE DATOS</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>160.2016906738281</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>METODOS MATEMATICOS II</t>
+          <t>CONTROL DE PROYECTOS</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>109</v>
+        <v>198.3759002685547</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ALGORITMIA</t>
+          <t>ESTADISTICA Y PROCESOS ESTOCASTICOS</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>106</v>
+        <v>355.6754760742188</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS I</t>
+          <t>ESTRUCTURAS DE DATOS I</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>61</v>
+        <v>38.69380187988281</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS II</t>
+          <t>ESTRUCTURAS DE DATOS II</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>129</v>
+        <v>75.54373168945312</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ADMINISTRACION DE REDES</t>
+          <t>HIPERMEDIA</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>74</v>
+        <v>195.336669921875</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ESTADISTICA Y PROCESOS ESTOCASTICOS</t>
+          <t>INGENIERIA DE SOFTWARE I</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>66</v>
+        <v>39.55695724487305</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ESTRUCTURAS DE DATOS II</t>
+          <t>INGENIERIA DE SOFTWARE II</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>11</v>
+        <v>139.5456237792969</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS II</t>
+          <t>METODOS MATEMATICOS I</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>80</v>
+        <v>323.9101257324219</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TEORIA DE LA COMPUTACION</t>
+          <t>METODOS MATEMATICOS II</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>79</v>
+        <v>286.1632995605469</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ADMINISTRACION DE SERVIDORES</t>
+          <t>MINERIA DE DATOS</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>87</v>
+        <v>160.5572967529297</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BASES DE DATOS</t>
+          <t>PROGRAMACION</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>63</v>
+        <v>269.4276428222656</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>HIPERMEDIA</t>
+          <t>PROGRAMACION PARA INTERNET</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>69</v>
+        <v>358.6423034667969</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>INGENIERIA DE SOFTWARE I</t>
+          <t>SEGURIDAD DE LA INFORMACION</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>30</v>
+        <v>196.5658569335938</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE BASES DE DATOS</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ALGORITMIA</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>116</v>
+        <v>270.6994018554688</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CONTROL DE PROYECTOS</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE BASES DE DATOS</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>88</v>
+        <v>232.9805603027344</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>INGENIERIA DE SOFTWARE II</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS I</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>82</v>
+        <v>35.28647613525391</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PROGRAMACION PARA INTERNET</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS II</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>169</v>
+        <v>138.6548919677734</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SEGURIDAD DE LA INFORMACION</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE INGENIERIA DE SOFTWARE I</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>119</v>
+        <v>281.482666015625</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE INGENIERIA DE SOFTWARE I</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS I</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>140</v>
+        <v>314.3976745605469</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE USO, ADAPTACION, EXPLOTACION DE SISTEMAS OPERATIVOS</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS II</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>122</v>
+        <v>307.2843017578125</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>USO, ADAPTACION Y EXPLOTACION DE SISTEMAS OPERATIVOS</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE PROGRAMACION</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>119</v>
+        <v>290.6789245605469</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ADMINISTRACION DE BASES DE DATOS</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE SISTEMAS BASADOS EN CONOCIMIENTO</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>101</v>
+        <v>126.8496170043945</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ALMACENES DE DATOS (DATA WAREHOUSE)</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE USO, ADAPTACION, EXPLOTACION DE SISTEMAS OPERATIVOS</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>75</v>
+        <v>177.7617034912109</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MINERIA DE DATOS</t>
+          <t>SISTEMAS BASADOS EN CONOCIMIENTO</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>101</v>
+        <v>134.867919921875</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CLASIFICACION INTELIGENTE DE DATOS</t>
+          <t>TEORIA DE LA COMPUTACION</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>88</v>
+        <v>58.2849006652832</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE SISTEMAS BASADOS EN CONOCIMIENTO</t>
+          <t>USO, ADAPTACION Y EXPLOTACION DE SISTEMAS OPERATIVOS</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>SISTEMAS BASADOS EN CONOCIMIENTO</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>113</v>
+        <v>160.5096130371094</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edited some parameters in Random Forest Notebook
</commit_message>
<xml_diff>
--- a/predicciones_cupos_proximo_semestre.xlsx
+++ b/predicciones_cupos_proximo_semestre.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>143.9074096679688</v>
+        <v>149.4883017415314</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>121.9426116943359</v>
+        <v>144.7113422432715</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>144.1614990234375</v>
+        <v>147.27590589659</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>133.6002960205078</v>
+        <v>145.7066161003521</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>151.3702545166016</v>
+        <v>148.8324072647092</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>152.0135345458984</v>
+        <v>155.1171063241644</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>160.2016906738281</v>
+        <v>153.6704701299099</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>198.3759002685547</v>
+        <v>198.6334567207135</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>355.6754760742188</v>
+        <v>362.1433803996547</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>38.69380187988281</v>
+        <v>68.70107168834457</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>75.54373168945312</v>
+        <v>73.56977806884662</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>195.336669921875</v>
+        <v>189.9157425227596</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>39.55695724487305</v>
+        <v>47.02370745953354</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>139.5456237792969</v>
+        <v>137.4376429993846</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>323.9101257324219</v>
+        <v>316.5360010704878</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>286.1632995605469</v>
+        <v>286.858166607642</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>160.5572967529297</v>
+        <v>149.182627445449</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>269.4276428222656</v>
+        <v>264.2715381946999</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>358.6423034667969</v>
+        <v>365.6947572331626</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>196.5658569335938</v>
+        <v>179.6626617176126</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>270.6994018554688</v>
+        <v>298.6928625621471</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>232.9805603027344</v>
+        <v>298.8082638992933</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>35.28647613525391</v>
+        <v>59.90295997935799</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>138.6548919677734</v>
+        <v>172.6149770563653</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>281.482666015625</v>
+        <v>284.0734371414941</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>314.3976745605469</v>
+        <v>336.2616647642</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>307.2843017578125</v>
+        <v>311.2186250419591</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>290.6789245605469</v>
+        <v>310.0406837930459</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>126.8496170043945</v>
+        <v>138.4669318193171</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>177.7617034912109</v>
+        <v>154.5108555958332</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>134.867919921875</v>
+        <v>139.5975827705442</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>58.2849006652832</v>
+        <v>74.28471843067288</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>160.5096130371094</v>
+        <v>147.2890190827495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A little improvement on the LSTM model
</commit_message>
<xml_diff>
--- a/predicciones_cupos_proximo_semestre.xlsx
+++ b/predicciones_cupos_proximo_semestre.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,334 +448,344 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADMINISTRACION DE BASES DE DATOS</t>
+          <t>MATEMATICA DISCRETA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>149.4883017415314</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ADMINISTRACION DE REDES</t>
+          <t>METODOS MATEMATICOS I</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>144.7113422432715</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ADMINISTRACION DE SERVIDORES</t>
+          <t>PROGRAMACION</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>147.27590589659</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ALGORITMIA</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE PROGRAMACION</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>145.7066161003521</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ALMACENES DE DATOS (DATA WAREHOUSE)</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS I</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>148.8324072647092</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BASES DE DATOS</t>
+          <t>ALGORITMIA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>155.1171063241644</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CLASIFICACION INTELIGENTE DE DATOS</t>
+          <t>ESTRUCTURAS DE DATOS I</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>153.6704701299099</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CONTROL DE PROYECTOS</t>
+          <t>METODOS MATEMATICOS II</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>198.6334567207135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ESTADISTICA Y PROCESOS ESTOCASTICOS</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ALGORITMIA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>362.1433803996547</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ESTRUCTURAS DE DATOS I</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS I</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>68.70107168834457</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ESTRUCTURAS DE DATOS II</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS II</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>73.56977806884662</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>HIPERMEDIA</t>
+          <t>ADMINISTRACION DE REDES</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>189.9157425227596</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>INGENIERIA DE SOFTWARE I</t>
+          <t>ESTADISTICA Y PROCESOS ESTOCASTICOS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>47.02370745953354</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>INGENIERIA DE SOFTWARE II</t>
+          <t>ESTRUCTURAS DE DATOS II</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>137.4376429993846</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>METODOS MATEMATICOS I</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS II</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>316.5360010704878</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>METODOS MATEMATICOS II</t>
+          <t>TEORIA DE LA COMPUTACION</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>286.858166607642</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MINERIA DE DATOS</t>
+          <t>ADMINISTRACION DE SERVIDORES</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>149.182627445449</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PROGRAMACION</t>
+          <t>BASES DE DATOS</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>264.2715381946999</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PROGRAMACION PARA INTERNET</t>
+          <t>HIPERMEDIA</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>365.6947572331626</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SEGURIDAD DE LA INFORMACION</t>
+          <t>INGENIERIA DE SOFTWARE I</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>179.6626617176126</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ALGORITMIA</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE BASES DE DATOS</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>298.6928625621471</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE BASES DE DATOS</t>
+          <t>CONTROL DE PROYECTOS</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>298.8082638992933</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS I</t>
+          <t>INGENIERIA DE SOFTWARE II</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>59.90295997935799</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS II</t>
+          <t>PROGRAMACION PARA INTERNET</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>172.6149770563653</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE INGENIERIA DE SOFTWARE I</t>
+          <t>SEGURIDAD DE LA INFORMACION</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>284.0734371414941</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS I</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE INGENIERIA DE SOFTWARE I</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>336.2616647642</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS II</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE USO, ADAPTACION, EXPLOTACION DE SISTEMAS OPERATIVOS</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>311.2186250419591</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE PROGRAMACION</t>
+          <t>USO, ADAPTACION Y EXPLOTACION DE SISTEMAS OPERATIVOS</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>310.0406837930459</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE SISTEMAS BASADOS EN CONOCIMIENTO</t>
+          <t>ADMINISTRACION DE BASES DE DATOS</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>138.4669318193171</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE USO, ADAPTACION, EXPLOTACION DE SISTEMAS OPERATIVOS</t>
+          <t>ALMACENES DE DATOS (DATA WAREHOUSE)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>154.5108555958332</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SISTEMAS BASADOS EN CONOCIMIENTO</t>
+          <t>MINERIA DE DATOS</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>139.5975827705442</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>TEORIA DE LA COMPUTACION</t>
+          <t>CLASIFICACION INTELIGENTE DE DATOS</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>74.28471843067288</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>USO, ADAPTACION Y EXPLOTACION DE SISTEMAS OPERATIVOS</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE SISTEMAS BASADOS EN CONOCIMIENTO</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>147.2890190827495</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>SISTEMAS BASADOS EN CONOCIMIENTO</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>